<commit_message>
criadas funções para cadastrar professores
</commit_message>
<xml_diff>
--- a/banco de dados.xlsx
+++ b/banco de dados.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\SFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA97EEE-0D26-4B3E-A0F9-70F3BB74E155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87970B05-1158-4589-90A5-2C302FE4D99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{83E668ED-BD3D-408E-97D4-730ABEA3C9B1}"/>
+    <workbookView xWindow="14295" yWindow="7740" windowWidth="14610" windowHeight="7845" xr2:uid="{83E668ED-BD3D-408E-97D4-730ABEA3C9B1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelas" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha3" sheetId="3" r:id="rId2"/>
+    <sheet name="Funções de cadastro" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,8 +26,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Lucas</author>
+  </authors>
+  <commentList>
+    <comment ref="O23" authorId="0" shapeId="0" xr:uid="{38004E44-747E-46BB-8A45-117A5ADFF51A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+O que identifica uma turma?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
   <si>
     <t>ALUNOS</t>
   </si>
@@ -69,9 +105,6 @@
     <t>id_aula</t>
   </si>
   <si>
-    <t>presenca</t>
-  </si>
-  <si>
     <t>assunto</t>
   </si>
   <si>
@@ -130,13 +163,85 @@
   </si>
   <si>
     <t>Aulas</t>
+  </si>
+  <si>
+    <t>presente</t>
+  </si>
+  <si>
+    <t>Funções okay:</t>
+  </si>
+  <si>
+    <t>cadastrar curso</t>
+  </si>
+  <si>
+    <t>cadastrar turma</t>
+  </si>
+  <si>
+    <t>control.py</t>
+  </si>
+  <si>
+    <t>modificar o verificar turma existe</t>
+  </si>
+  <si>
+    <t>Cadastrar Aluno</t>
+  </si>
+  <si>
+    <t>Cadastrar Curso</t>
+  </si>
+  <si>
+    <t>Nome do curso</t>
+  </si>
+  <si>
+    <t>Cadastrar Turma</t>
+  </si>
+  <si>
+    <t>Nome da turma</t>
+  </si>
+  <si>
+    <t>Curso</t>
+  </si>
+  <si>
+    <t>Turno</t>
+  </si>
+  <si>
+    <t>Dia da semana</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Telefone</t>
+  </si>
+  <si>
+    <t>Dados que precisam para cadastrar</t>
+  </si>
+  <si>
+    <t>Cadastrar Aula</t>
+  </si>
+  <si>
+    <t>Cadastrar Professor</t>
+  </si>
+  <si>
+    <t>Nome do professor</t>
+  </si>
+  <si>
+    <t>Assunto</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Turma</t>
+  </si>
+  <si>
+    <t>Data_cadastro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,8 +257,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,8 +358,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -269,11 +401,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -326,6 +503,22 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,6 +544,72 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFC94DF2-DE24-9780-CB15-43B0322193AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3171825" y="2409825"/>
+          <a:ext cx="1828800" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
@@ -669,6 +928,138 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Retângulo 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BD725D9-D9BB-1199-C8B2-38C8079CEDEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1647825" y="2047875"/>
+          <a:ext cx="1133475" cy="1285874"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Retângulo 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89F0856D-B369-AD0E-51B0-7A8DD2B3350D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="238125" y="1104900"/>
+          <a:ext cx="1028700" cy="1447800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -968,11 +1359,240 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33787AD1-B3CC-4EA7-9557-11A644423C87}">
-  <dimension ref="A1:O28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33787AD1-B3CC-4EA7-9557-11A644423C87}">
+  <dimension ref="B5:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="11" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="11" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="11" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.42578125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" style="11"/>
+    <col min="13" max="13" width="19.7109375" style="11" customWidth="1"/>
+    <col min="14" max="14" width="26.85546875" style="11" customWidth="1"/>
+    <col min="15" max="15" width="17" style="11" customWidth="1"/>
+    <col min="16" max="16" width="5.42578125" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D17" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M21" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M22" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="N22" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M23" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="N23" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="O23" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E24" s="19"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="19"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D445F4E7-94C2-4E7A-B836-C8B335E68544}">
+  <dimension ref="A1:K27"/>
+  <sheetViews>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection sqref="A1:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,40 +1608,41 @@
     <col min="9" max="9" width="2.42578125" style="11" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.140625" style="11"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" customWidth="1"/>
     <col min="14" max="14" width="26.85546875" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" customWidth="1"/>
+    <col min="16" max="16" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
       <c r="B1" s="11"/>
       <c r="D1" s="11"/>
       <c r="F1" s="11"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="D2" s="11"/>
       <c r="F2" s="11"/>
       <c r="H2" s="11"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="D3" s="11"/>
       <c r="F3" s="11"/>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="D4" s="11"/>
       <c r="F4" s="11"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -1033,20 +1654,12 @@
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
-      <c r="M5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
-      <c r="D6" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -1054,152 +1667,90 @@
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
-      <c r="M6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
-      <c r="B7" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="B7" s="2"/>
       <c r="C7" s="10"/>
-      <c r="D7" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="10"/>
-      <c r="F7" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
-      <c r="M7" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
-      <c r="B8" s="17" t="s">
-        <v>6</v>
-      </c>
+      <c r="B8" s="17"/>
       <c r="C8" s="10"/>
-      <c r="D8" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="D8" s="8"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="16" t="s">
-        <v>6</v>
-      </c>
+      <c r="F8" s="16"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="10"/>
-      <c r="D9" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="D9" s="4"/>
       <c r="E9" s="10"/>
-      <c r="F9" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
-      <c r="M9" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B10" s="1"/>
       <c r="C10" s="10"/>
-      <c r="D10" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="F10" s="1"/>
       <c r="G10" s="10"/>
-      <c r="H10" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="H10" s="2"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
-      <c r="M10" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
-      <c r="B11" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="F11" s="5"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="15" t="s">
-        <v>6</v>
-      </c>
+      <c r="H11" s="15"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
-      <c r="B12" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="B12" s="7"/>
       <c r="C12" s="10"/>
-      <c r="D12" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="F12" s="7"/>
       <c r="G12" s="10"/>
-      <c r="H12" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="H12" s="1"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="C13" s="10"/>
-      <c r="D13" s="14" t="s">
-        <v>6</v>
-      </c>
+      <c r="D13" s="14"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
@@ -1208,93 +1759,158 @@
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D14" s="1"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="F14" s="2"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
     </row>
-    <row r="15" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
-      <c r="D15" s="13" t="s">
-        <v>18</v>
-      </c>
+      <c r="D15" s="13"/>
       <c r="E15" s="10"/>
-      <c r="F15" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="F15" s="6"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
-      <c r="D16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D16" s="1"/>
+      <c r="F16" s="1"/>
       <c r="H16" s="11"/>
     </row>
-    <row r="17" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="4:5" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E24" s="19"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>25</v>
-      </c>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D27" s="18"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>26</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169C44E6-C184-4706-A188-038D9401FB57}">
+  <dimension ref="B1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="11" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="4" spans="2:8" s="22" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
pequenos ajustes no model
</commit_message>
<xml_diff>
--- a/banco de dados.xlsx
+++ b/banco de dados.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\SFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87970B05-1158-4589-90A5-2C302FE4D99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856CCBAE-4A67-4644-9042-3C391C7E586F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="7740" windowWidth="14610" windowHeight="7845" xr2:uid="{83E668ED-BD3D-408E-97D4-730ABEA3C9B1}"/>
+    <workbookView xWindow="17070" yWindow="5535" windowWidth="11835" windowHeight="10050" activeTab="1" xr2:uid="{83E668ED-BD3D-408E-97D4-730ABEA3C9B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelas" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha3" sheetId="3" r:id="rId2"/>
-    <sheet name="Funções de cadastro" sheetId="2" r:id="rId3"/>
+    <sheet name="Funções de cadastro" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +31,7 @@
     <author>Lucas</author>
   </authors>
   <commentList>
-    <comment ref="O23" authorId="0" shapeId="0" xr:uid="{38004E44-747E-46BB-8A45-117A5ADFF51A}">
+    <comment ref="L23" authorId="0" shapeId="0" xr:uid="{38004E44-747E-46BB-8A45-117A5ADFF51A}">
       <text>
         <r>
           <rPr>
@@ -52,7 +51,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-O que identifica uma turma?</t>
+O que identifica uma turma?
+nome</t>
         </r>
       </text>
     </comment>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
   <si>
     <t>ALUNOS</t>
   </si>
@@ -132,9 +132,6 @@
     <t>e retornar grade</t>
   </si>
   <si>
-    <t>apagar banco de dados e testa cadastro</t>
-  </si>
-  <si>
     <t>turma tem q verificar nome diferente tbm</t>
   </si>
   <si>
@@ -235,13 +232,40 @@
   </si>
   <si>
     <t>Data_cadastro</t>
+  </si>
+  <si>
+    <t>cadastrar aluno</t>
+  </si>
+  <si>
+    <t>script</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>Cadastro</t>
+  </si>
+  <si>
+    <t>Cursos</t>
+  </si>
+  <si>
+    <t>Turmas</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Presencas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +275,14 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -450,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -458,9 +490,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -501,22 +530,30 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -547,15 +584,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:colOff>473766</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>148673</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>57978</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>33131</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -570,8 +607,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3171825" y="2409825"/>
-          <a:ext cx="1828800" cy="762000"/>
+          <a:off x="3182179" y="2434673"/>
+          <a:ext cx="1795669" cy="646458"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -931,15 +968,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
+      <xdr:colOff>496957</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>165652</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:colOff>24848</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:rowOff>33130</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -954,8 +991,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1647825" y="2047875"/>
-          <a:ext cx="1133475" cy="1285874"/>
+          <a:off x="1697935" y="2070652"/>
+          <a:ext cx="1035326" cy="1200978"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -997,15 +1034,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:colOff>256761</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:colOff>41413</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>33130</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1020,8 +1057,226 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="238125" y="1104900"/>
-          <a:ext cx="1028700" cy="1447800"/>
+          <a:off x="256761" y="1104900"/>
+          <a:ext cx="985630" cy="1404730"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>364434</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>140804</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>41413</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>41413</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Retângulo 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B76C0B33-9D5D-AC3E-9D4A-9F1505E272DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5284304" y="1664804"/>
+          <a:ext cx="977348" cy="662609"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>274983</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>41000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>140804</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>140804</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Retângulo 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E461DAC9-C51D-2DD6-8828-E9C76ED127DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="581440" y="5184500"/>
+          <a:ext cx="2267777" cy="861804"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>no</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> control.py a função de cadastro está okay</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>473766</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>110573</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57978</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Retângulo 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D96ED14-6338-C0CF-C83B-E7EC3BB3C57C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3188391" y="1063073"/>
+          <a:ext cx="1794012" cy="1270552"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1360,55 +1615,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33787AD1-B3CC-4EA7-9557-11A644423C87}">
-  <dimension ref="B5:O28"/>
+  <dimension ref="B5:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="11" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="11" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="11" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.42578125" style="11" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="11"/>
-    <col min="13" max="13" width="19.7109375" style="11" customWidth="1"/>
-    <col min="14" max="14" width="26.85546875" style="11" customWidth="1"/>
-    <col min="15" max="15" width="17" style="11" customWidth="1"/>
-    <col min="16" max="16" width="5.42578125" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="1" width="4.5703125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="10" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.42578125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="10" customWidth="1"/>
+    <col min="11" max="11" width="21" style="10" customWidth="1"/>
+    <col min="12" max="12" width="24.28515625" style="10" customWidth="1"/>
+    <col min="13" max="13" width="36" style="10" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="M5" s="10" t="s">
+    <row r="5" spans="2:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N5" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L5" s="11"/>
+    </row>
+    <row r="6" spans="2:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="J6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="L6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
@@ -1418,41 +1672,48 @@
       <c r="F7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
+      <c r="J7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+    </row>
+    <row r="8" spans="2:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" spans="2:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="2:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>15</v>
@@ -1460,44 +1721,46 @@
       <c r="H10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M10" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="J10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="2:12" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+    <row r="12" spans="2:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1505,15 +1768,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="13" t="s">
+    <row r="15" spans="2:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1521,64 +1784,143 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D17" s="12" t="s">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D17" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="11" t="s">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="M21" s="11" t="s">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J21" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" s="18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="M22" s="11" t="s">
+      <c r="K22" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="N22" s="11" t="s">
+      <c r="K23" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="L23" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M23" s="11" t="s">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E24" s="17"/>
+      <c r="J24" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K24" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="N23" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="O23" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E24" s="19"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="19"/>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
-        <v>25</v>
-      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D27" s="17"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1588,323 +1930,103 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D445F4E7-94C2-4E7A-B836-C8B335E68544}">
-  <dimension ref="A1:K27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169C44E6-C184-4706-A188-038D9401FB57}">
+  <dimension ref="B1:H8"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection sqref="A1:J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="11" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="11" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.42578125" style="11" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="11"/>
-    <col min="13" max="13" width="19.7109375" customWidth="1"/>
-    <col min="14" max="14" width="26.85546875" customWidth="1"/>
-    <col min="15" max="15" width="17" customWidth="1"/>
-    <col min="16" max="16" width="5.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="H1" s="11"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="H2" s="11"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="H3" s="11"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="H4" s="11"/>
-    </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-    </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-    </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-    </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-    </row>
-    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-    </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-    </row>
-    <row r="11" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-    </row>
-    <row r="12" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-    </row>
-    <row r="13" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-    </row>
-    <row r="14" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-    </row>
-    <row r="15" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="D16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="H16" s="11"/>
-    </row>
-    <row r="17" spans="4:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="12"/>
-    </row>
-    <row r="18" spans="4:5" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="19"/>
-    </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D27" s="18"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169C44E6-C184-4706-A188-038D9401FB57}">
-  <dimension ref="B1:H8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.28515625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="4.28515625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="4.85546875" style="11" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="11" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="1" width="5.28515625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" style="10" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="10" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="4" spans="2:8" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
-    </row>
-    <row r="4" spans="2:8" s="22" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="s">
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="21" t="s">
+      <c r="F5" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="20" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D6" s="20" t="s">
+      <c r="D7" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="20" t="s">
+      <c r="F7" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D8" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>32</v>
+      <c r="F8" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
visualização melhorada da seleção de turmas para gera grade
</commit_message>
<xml_diff>
--- a/banco de dados.xlsx
+++ b/banco de dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\SFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856CCBAE-4A67-4644-9042-3C391C7E586F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBDB088-C22E-47DD-9066-C1ABA2179BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17070" yWindow="5535" windowWidth="11835" windowHeight="10050" activeTab="1" xr2:uid="{83E668ED-BD3D-408E-97D4-730ABEA3C9B1}"/>
+    <workbookView xWindow="5085" yWindow="1395" windowWidth="18945" windowHeight="11295" xr2:uid="{83E668ED-BD3D-408E-97D4-730ABEA3C9B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelas" sheetId="1" r:id="rId1"/>
@@ -541,6 +541,12 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -548,12 +554,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1617,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33787AD1-B3CC-4EA7-9557-11A644423C87}">
   <dimension ref="B5:L43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1861,66 +1861,66 @@
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="C38" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="26" t="s">
+      <c r="D38" s="23" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="26" t="s">
+      <c r="D39" s="23" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="26" t="s">
+      <c r="C40" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D40" s="26" t="s">
+      <c r="D40" s="23" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="25" t="s">
+      <c r="B41" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="26" t="s">
+      <c r="C41" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D41" s="26" t="s">
+      <c r="D41" s="23" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="26" t="s">
+      <c r="C42" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="26" t="s">
+      <c r="D42" s="23" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="25" t="s">
+      <c r="B43" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1933,7 +1933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169C44E6-C184-4706-A188-038D9401FB57}">
   <dimension ref="B1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -1952,15 +1952,15 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="4" spans="2:8" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">

</xml_diff>

<commit_message>
falta ajeitar a grade
</commit_message>
<xml_diff>
--- a/banco de dados.xlsx
+++ b/banco de dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\SFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBDB088-C22E-47DD-9066-C1ABA2179BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1380C2-1A79-47FB-A384-F3433334F46A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="1395" windowWidth="18945" windowHeight="11295" xr2:uid="{83E668ED-BD3D-408E-97D4-730ABEA3C9B1}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
   <si>
     <t>ALUNOS</t>
   </si>
@@ -123,21 +123,12 @@
     <t>dia_semana</t>
   </si>
   <si>
-    <t>Está dando um erro ao salvar aulas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e retornar assunto </t>
-  </si>
-  <si>
     <t>e retornar grade</t>
   </si>
   <si>
     <t>turma tem q verificar nome diferente tbm</t>
   </si>
   <si>
-    <t>afinal podem existir duas turmas ai mesmo tempo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cursos: </t>
   </si>
   <si>
@@ -259,6 +250,12 @@
   </si>
   <si>
     <t>Presencas</t>
+  </si>
+  <si>
+    <t>afinal podem existir duas turmas ao mesmo tempo</t>
+  </si>
+  <si>
+    <t>apresentação da grade da aula</t>
   </si>
 </sst>
 </file>
@@ -1617,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33787AD1-B3CC-4EA7-9557-11A644423C87}">
   <dimension ref="B5:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1641,10 +1638,10 @@
   <sheetData>
     <row r="5" spans="2:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="J5" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L5" s="11"/>
     </row>
@@ -1653,13 +1650,13 @@
         <v>5</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1673,7 +1670,7 @@
         <v>3</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
@@ -1703,7 +1700,7 @@
         <v>14</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
@@ -1713,7 +1710,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>15</v>
@@ -1722,7 +1719,7 @@
         <v>4</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
@@ -1789,61 +1786,56 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="J21" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="K21" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J22" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="K22" s="18" t="s">
         <v>34</v>
-      </c>
-      <c r="K21" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J22" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="K22" s="18" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K23" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E24" s="17"/>
       <c r="J24" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
@@ -1851,73 +1843,73 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="22" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C43" s="23"/>
       <c r="D43" s="23"/>
@@ -1953,7 +1945,7 @@
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
@@ -1964,69 +1956,69 @@
     </row>
     <row r="4" spans="2:8" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D6" s="18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>55</v>
-      </c>
       <c r="H8" s="18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>